<commit_message>
update teacher class record
</commit_message>
<xml_diff>
--- a/frontend/public/templates/students_list.xlsx
+++ b/frontend/public/templates/students_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\NihonStudyGuide\frontend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CFA28D-3ECB-4AEC-AE3A-B9A9539EEE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F9C57E-0B05-4597-A1C0-3AB455421BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{56EDAB6C-C3B7-4DDE-92F9-23A04AE68FED}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>